<commit_message>
fixed NC alphas and betas in input file
</commit_message>
<xml_diff>
--- a/NC_Data/NC 2016 statewide alpha and beta calculation.xlsx
+++ b/NC_Data/NC 2016 statewide alpha and beta calculation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mira/Dropbox (Mathcamp)/EI/Pyro/eipython/NC_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mira/Dropbox (Mathcamp)/eipython/NC_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="11140" windowHeight="16660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Computing alpha and beta" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
-  <si>
-    <t>Raw data based on:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
     <t>var</t>
   </si>
@@ -141,13 +138,22 @@
     <t>test that it works: take exp and compute column sum</t>
   </si>
   <si>
-    <t>column sum</t>
+    <t>Yay, it works!</t>
   </si>
   <si>
-    <t>divide by column sum</t>
+    <t>Raw data from:</t>
   </si>
   <si>
-    <t>Yay, it works!</t>
+    <t>row sum</t>
+  </si>
+  <si>
+    <t>divide by row sum</t>
+  </si>
+  <si>
+    <t>In the input tab, the candidates are: 0 (other), 1 (Dem), 2 (Rep)</t>
+  </si>
+  <si>
+    <t>the races are: 0 (white), 1 (black), 2(other)</t>
   </si>
 </sst>
 </file>
@@ -452,13 +458,13 @@
   </sheetPr>
   <dimension ref="A1:AB1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="30.5" customWidth="1"/>
     <col min="10" max="10" width="29.6640625" customWidth="1"/>
     <col min="11" max="11" width="27.5" customWidth="1"/>
@@ -466,10 +472,10 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
@@ -496,7 +502,7 @@
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9"/>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -548,16 +554,16 @@
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F4" s="7"/>
       <c r="L4" s="10"/>
@@ -580,7 +586,7 @@
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>0.32</v>
@@ -615,7 +621,7 @@
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>0.89</v>
@@ -650,7 +656,7 @@
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>0.56000000000000005</v>
@@ -707,7 +713,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -748,13 +754,13 @@
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="11"/>
@@ -773,7 +779,7 @@
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="9">
         <f t="shared" ref="B12:B14" si="0">E5*B5</f>
@@ -804,7 +810,7 @@
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="9">
         <f t="shared" si="0"/>
@@ -835,7 +841,7 @@
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="9">
         <f t="shared" si="0"/>
@@ -893,7 +899,7 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -944,13 +950,13 @@
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="11"/>
@@ -974,7 +980,7 @@
     </row>
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="9">
         <f t="shared" ref="B19:D19" si="3">LN(B12)</f>
@@ -1010,7 +1016,7 @@
     </row>
     <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="9">
         <f t="shared" ref="B20:D20" si="4">LN(B13)</f>
@@ -1046,7 +1052,7 @@
     </row>
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="9">
         <f t="shared" ref="B21:D21" si="5">LN(B14)</f>
@@ -1090,7 +1096,7 @@
         <v>-1.2555976547314274</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1139,7 +1145,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1190,13 +1196,13 @@
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="D26" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" s="11"/>
       <c r="L26" s="3"/>
@@ -1219,7 +1225,7 @@
     </row>
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="9">
         <f t="shared" ref="B27:D27" si="6">B19-$E$22</f>
@@ -1255,7 +1261,7 @@
     </row>
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="9">
         <f t="shared" ref="B28:D28" si="7">B20-$E$22</f>
@@ -1291,7 +1297,7 @@
     </row>
     <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="9">
         <f t="shared" ref="B29:D29" si="8">B21-$E$22</f>
@@ -1327,7 +1333,7 @@
     </row>
     <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="14">
         <f t="shared" ref="B30:D30" si="9">AVERAGE(B27:B29)</f>
@@ -1346,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -1395,7 +1401,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="3"/>
@@ -1455,16 +1461,16 @@
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="11"/>
@@ -1493,7 +1499,7 @@
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="16">
         <f t="shared" ref="B35:D35" si="10">B27-B$30</f>
@@ -1534,7 +1540,7 @@
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="16">
         <f t="shared" ref="B36:D36" si="11">B28-B$30</f>
@@ -1575,7 +1581,7 @@
     </row>
     <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="16">
         <f t="shared" ref="B37:D37" si="12">B29-B$30</f>
@@ -1630,7 +1636,7 @@
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1689,7 +1695,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1750,16 +1756,16 @@
     <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D42" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="3"/>
@@ -1787,7 +1793,7 @@
     </row>
     <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43" s="9">
         <f t="shared" ref="B43:D43" si="14">EXP(B$30+B35)</f>
@@ -1831,7 +1837,7 @@
     </row>
     <row r="44" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" s="9">
         <f t="shared" ref="B44:D44" si="16">EXP(B$30+B36)</f>
@@ -1875,7 +1881,7 @@
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="9">
         <f t="shared" ref="B45:D45" si="17">EXP(B$30+B37)</f>
@@ -1951,7 +1957,7 @@
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -2012,13 +2018,13 @@
     <row r="49" spans="1:28" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
       <c r="B49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="11"/>
@@ -2047,7 +2053,7 @@
     </row>
     <row r="50" spans="1:28" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B50" s="9">
         <f t="shared" ref="B50:D50" si="18">B43/$E43</f>
@@ -2088,7 +2094,7 @@
     </row>
     <row r="51" spans="1:28" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" s="9">
         <f t="shared" ref="B51:D51" si="19">B44/$E44</f>
@@ -2129,7 +2135,7 @@
     </row>
     <row r="52" spans="1:28" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B52" s="9">
         <f t="shared" ref="B52:D52" si="20">B45/$E45</f>
@@ -2202,7 +2208,7 @@
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -2291,7 +2297,9 @@
       <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="3"/>
+      <c r="A57" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2322,7 +2330,9 @@
     </row>
     <row r="58" spans="1:28" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
+      <c r="B58" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
@@ -30746,28 +30756,30 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -30775,24 +30787,24 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>0.2</v>
+      <c r="E2">
+        <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>-0.48</v>
+        <v>0.2</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -30801,13 +30813,13 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2">
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>0.28000000000000003</v>
+        <v>-0.48</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -30816,7 +30828,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -30834,7 +30846,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -30852,7 +30864,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -30870,7 +30882,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -30887,7 +30899,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -30905,7 +30917,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -30919,7 +30931,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -30933,7 +30945,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -30947,7 +30959,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>

</xml_diff>